<commit_message>
edit config json file
</commit_message>
<xml_diff>
--- a/TestData/login.xlsx
+++ b/TestData/login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Playwright\Playwright_TypeScript\Playwright_TS_Cucumber\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D6304E-13EA-468F-98C6-410D669847F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4CF9C8-6A41-461B-9AB3-2382133AC2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>abcjsjs@gmail.com</t>
+  </si>
+  <si>
+    <t>jxbsansanas</t>
   </si>
 </sst>
 </file>
@@ -96,13 +99,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -387,7 +393,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -405,8 +411,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>